<commit_message>
cambios en biometrias y nutricion
</commit_message>
<xml_diff>
--- a/files/reports/nutricion/reporte_nutricion.xlsx
+++ b/files/reports/nutricion/reporte_nutricion.xlsx
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,14 +118,6 @@
       <sz val="24"/>
       <color theme="8" tint="-0.499984740745262"/>
       <name val="Roboto"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="8" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -243,9 +235,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -271,6 +260,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -606,7 +598,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -623,113 +615,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="19" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="11" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="11"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="11"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="11"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="11"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="11"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="11"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
       <c r="B8" s="4"/>
@@ -746,38 +738,38 @@
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="J9" s="12" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="J9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="10"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="J10" s="12" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="J10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="10"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">

</xml_diff>